<commit_message>
create sheet and option
</commit_message>
<xml_diff>
--- a/Sentiment/Sentiment.Services/download.xlsx
+++ b/Sentiment/Sentiment.Services/download.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Style" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Style" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -339,22 +339,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>